<commit_message>
Cambios y arreglos menores
1-Se agrego soporte para poder trabajar con la version de avion RPB.
2- Ya se desmarca el color de las piezas que fueron eliminadas
</commit_message>
<xml_diff>
--- a/Created_records.xlsx
+++ b/Created_records.xlsx
@@ -424,7 +424,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B14" sqref="B14"/>
@@ -472,6 +472,30 @@
         </is>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Avion3</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>v1000</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Version RPB</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>RPB</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>

<commit_message>
Se guarda el cuadrante de la pieza en el excel
</commit_message>
<xml_diff>
--- a/Created_records.xlsx
+++ b/Created_records.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luisg\Documents\Python Projects\DIGITALIZACION_DE_CALIDAD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79A08ECD-7353-4A14-97A5-89FA1D46F4A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A9555A3-B22D-4331-AAC2-3892D7A97EAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="480" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5085" yWindow="4020" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>record_name</t>
   </si>
@@ -31,13 +31,7 @@
     <t>v900</t>
   </si>
   <si>
-    <t>v1000</t>
-  </si>
-  <si>
-    <t>Nueva ver</t>
-  </si>
-  <si>
-    <t>Nueva ver v1000</t>
+    <t>Test1</t>
   </si>
 </sst>
 </file>
@@ -389,10 +383,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -411,18 +405,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B2" t="s">
         <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" t="s">
-        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>